<commit_message>
worked on intertemporal exporter codes and notes
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/importer-iiso3n_intertemporal_countrycode_adjustments.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/importer-iiso3n_intertemporal_countrycode_adjustments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="183">
   <si>
     <t>coverage</t>
   </si>
@@ -460,9 +460,6 @@
     <t>1972-2000</t>
   </si>
   <si>
-    <t>Interpolate</t>
-  </si>
-  <si>
     <t>1969-2000</t>
   </si>
   <si>
@@ -475,27 +472,18 @@
     <t>CSK-CZESVK</t>
   </si>
   <si>
-    <t>DROP. No real natural alignment</t>
-  </si>
-  <si>
     <t>DEU-DDRDEU</t>
   </si>
   <si>
     <t>Alternatives</t>
   </si>
   <si>
-    <t>INDBGD</t>
-  </si>
-  <si>
     <t>YEMYMD-YEM</t>
   </si>
   <si>
     <t>SPLIT</t>
   </si>
   <si>
-    <t>MERGE; RECODE: YEM</t>
-  </si>
-  <si>
     <t>YUG-BIHHRVMKDMNESVNSRB</t>
   </si>
   <si>
@@ -542,6 +530,39 @@
   </si>
   <si>
     <t>Technically Rhodesia</t>
+  </si>
+  <si>
+    <t>IND-INDBGD</t>
+  </si>
+  <si>
+    <t>DROP or ADD to FRA</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>INTERPOLATE?</t>
+  </si>
+  <si>
+    <t>COLLAPSE</t>
+  </si>
+  <si>
+    <t>INTERPOLATE</t>
+  </si>
+  <si>
+    <t>Merge with CHN</t>
+  </si>
+  <si>
+    <t>DROP?</t>
+  </si>
+  <si>
+    <t>1993-2000</t>
+  </si>
+  <si>
+    <t>MERGE</t>
   </si>
 </sst>
 </file>
@@ -606,36 +627,114 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -939,12 +1038,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU51"/>
+  <dimension ref="A1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3195" topLeftCell="S1" activePane="topRight"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2745" topLeftCell="AI1" activePane="topRight"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="topRight" activeCell="AT21" sqref="AT21"/>
+      <selection pane="topRight" activeCell="AU51" sqref="AU51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +1056,11 @@
     <col min="44" max="44" width="3.5703125" customWidth="1"/>
     <col min="45" max="45" width="2.28515625" customWidth="1"/>
     <col min="46" max="46" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="41.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="D1" s="1">
         <v>1962</v>
       </c>
@@ -1084,14 +1184,20 @@
       <c r="AR1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="AU1" s="9" t="s">
-        <v>155</v>
+      <c r="AU1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AW1" s="11" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1101,9 +1207,9 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AT2" s="4"/>
+      <c r="AT2" s="3"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1176,14 +1282,20 @@
       <c r="AR3" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT3" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU3" s="7" t="s">
+      <c r="AT3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU3" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW3" s="14" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1256,14 +1368,20 @@
       <c r="AR4" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT4" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU4" s="7" t="s">
+      <c r="AT4" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU4" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV4" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW4" s="14" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1376,14 +1494,20 @@
       <c r="AR5" s="2">
         <v>0.74358974358974395</v>
       </c>
-      <c r="AT5" s="7" t="s">
+      <c r="AT5" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AU5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AU5" s="6" t="s">
-        <v>156</v>
+      <c r="AV5" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW5" s="14" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1456,14 +1580,20 @@
       <c r="AR6" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT6" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU6" s="7" t="s">
+      <c r="AT6" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU6" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV6" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW6" s="14" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1592,12 +1722,14 @@
       <c r="AR7" s="2">
         <v>0.94871794871794901</v>
       </c>
-      <c r="AT7" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU7" s="6"/>
+      <c r="AT7" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW7" s="14" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1670,14 +1802,20 @@
       <c r="AR8" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT8" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AU8" s="6" t="s">
+      <c r="AT8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU8" s="18" t="s">
         <v>146</v>
       </c>
+      <c r="AV8" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW8" s="18" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1802,14 +1940,14 @@
       <c r="AR9" s="2">
         <v>0.89743589743589702</v>
       </c>
-      <c r="AT9" s="7" t="s">
+      <c r="AT9" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="AU9" s="6" t="s">
-        <v>150</v>
+      <c r="AU9" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1868,12 +2006,14 @@
       <c r="AR10" s="2">
         <v>5.1282051282051301E-2</v>
       </c>
-      <c r="AT10" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU10" s="6"/>
+      <c r="AT10" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU10" s="19" t="s">
+        <v>179</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1946,14 +2086,20 @@
       <c r="AR11" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT11" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AU11" s="6" t="s">
+      <c r="AT11" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU11" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV11" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW11" s="20" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2024,14 +2170,20 @@
       <c r="AR12" s="2">
         <v>0.20512820512820501</v>
       </c>
-      <c r="AT12" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU12" s="6" t="s">
-        <v>158</v>
+      <c r="AT12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU12" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="AV12" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW12" s="21" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -2148,14 +2300,17 @@
       <c r="AR13" s="2">
         <v>0.79487179487179505</v>
       </c>
-      <c r="AT13" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU13" s="6" t="s">
-        <v>158</v>
+      <c r="AT13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AV13" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW13" s="21" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2228,12 +2383,20 @@
       <c r="AR14" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT14" s="7" t="s">
+      <c r="AT14" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU14" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AU14" s="6"/>
+      <c r="AV14" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW14" s="22" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -2350,12 +2513,16 @@
       <c r="AR15" s="2">
         <v>0.79487179487179505</v>
       </c>
-      <c r="AT15" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AU15" s="6"/>
+      <c r="AT15" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="AU15" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="AV15" s="23"/>
+      <c r="AW15" s="23"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -2468,12 +2635,17 @@
       <c r="AR16" s="2">
         <v>0.74358974358974395</v>
       </c>
-      <c r="AT16" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU16" s="6"/>
+      <c r="AT16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV16" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW16" s="26" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2586,11 +2758,17 @@
       <c r="AR17" s="2">
         <v>0.74358974358974395</v>
       </c>
-      <c r="AT17" s="7" t="s">
-        <v>154</v>
+      <c r="AT17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV17" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW17" s="26" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2705,11 +2883,11 @@
       <c r="AR18" s="2">
         <v>0.76923076923076905</v>
       </c>
-      <c r="AT18" s="10" t="s">
-        <v>161</v>
+      <c r="AT18" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -2822,14 +3000,18 @@
       <c r="AR19" s="2">
         <v>0.74358974358974395</v>
       </c>
-      <c r="AT19" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>159</v>
+      <c r="AT19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU19" s="27"/>
+      <c r="AV19" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW19" s="28" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2886,15 +3068,19 @@
       <c r="AR20" s="2">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="AT20" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU20" s="6" t="s">
-        <v>159</v>
+      <c r="AT20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU20" s="27"/>
+      <c r="AV20" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW20" s="28" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3006,15 +3192,19 @@
       <c r="AR21" s="2">
         <v>0.74358974358974395</v>
       </c>
-      <c r="AT21" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU21" s="6" t="s">
-        <v>159</v>
+      <c r="AT21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU21" s="29"/>
+      <c r="AV21" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW21" s="30" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>69</v>
       </c>
@@ -3068,14 +3258,18 @@
       <c r="AR22" s="2">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="AT22" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AU22" s="6" t="s">
-        <v>159</v>
+      <c r="AT22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU22" s="29"/>
+      <c r="AV22" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW22" s="30" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -3190,14 +3384,18 @@
       <c r="AR23" s="2">
         <v>0.76923076923076905</v>
       </c>
-      <c r="AT23" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>158</v>
+      <c r="AT23" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU23" s="31"/>
+      <c r="AV23" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW23" s="32" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -3328,14 +3526,14 @@
       <c r="AR24" s="2">
         <v>0.97435897435897401</v>
       </c>
-      <c r="AT24" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU24" s="11" t="s">
-        <v>165</v>
+      <c r="AT24" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU24" s="16" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -3408,14 +3606,20 @@
       <c r="AR25" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT25" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU25" s="7" t="s">
+      <c r="AT25" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU25" s="33" t="s">
         <v>146</v>
       </c>
+      <c r="AV25" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW25" s="33" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -3490,14 +3694,20 @@
       <c r="AR26" s="2">
         <v>0.256410256410256</v>
       </c>
-      <c r="AT26" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU26" s="7" t="s">
-        <v>163</v>
+      <c r="AT26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU26" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="AV26" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW26" s="34" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -3626,11 +3836,11 @@
       <c r="AR27" s="2">
         <v>0.94871794871794901</v>
       </c>
-      <c r="AT27" s="8" t="s">
-        <v>148</v>
+      <c r="AT27" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -3761,14 +3971,14 @@
       <c r="AR28" s="2">
         <v>0.97435897435897401</v>
       </c>
-      <c r="AT28" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU28" s="11" t="s">
-        <v>165</v>
+      <c r="AT28" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU28" s="16" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -3899,14 +4109,14 @@
       <c r="AR29" s="2">
         <v>0.97435897435897401</v>
       </c>
-      <c r="AT29" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU29" s="11" t="s">
-        <v>165</v>
+      <c r="AT29" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU29" s="16" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -3979,14 +4189,20 @@
       <c r="AR30" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT30" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU30" s="7" t="s">
+      <c r="AT30" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU30" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV30" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW30" s="35" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -4059,14 +4275,20 @@
       <c r="AR31" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT31" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU31" s="7" t="s">
+      <c r="AT31" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU31" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV31" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW31" s="35" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -4139,14 +4361,20 @@
       <c r="AR32" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT32" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU32" s="7" t="s">
+      <c r="AT32" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU32" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV32" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW32" s="35" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -4219,14 +4447,20 @@
       <c r="AR33" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT33" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU33" s="7" t="s">
+      <c r="AT33" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU33" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV33" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW33" s="35" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -4355,14 +4589,14 @@
       <c r="AR34" s="2">
         <v>0.94871794871794901</v>
       </c>
-      <c r="AT34" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="AU34" s="7" t="s">
-        <v>167</v>
+      <c r="AT34" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU34" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -4419,11 +4653,11 @@
       <c r="AR35" s="2">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="AT35" s="10" t="s">
-        <v>168</v>
+      <c r="AT35" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -4496,14 +4730,20 @@
       <c r="AR36" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT36" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU36" s="7" t="s">
+      <c r="AT36" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU36" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV36" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW36" s="36" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -4568,14 +4808,20 @@
       <c r="AR37" s="2">
         <v>0.128205128205128</v>
       </c>
-      <c r="AT37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU37" s="7" t="s">
-        <v>162</v>
+      <c r="AT37" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU37" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="AV37" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW37" s="36" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -4706,11 +4952,11 @@
       <c r="AR38" s="2">
         <v>0.97435897435897401</v>
       </c>
-      <c r="AT38" s="12" t="s">
-        <v>169</v>
+      <c r="AT38" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -4837,11 +5083,14 @@
       <c r="AR39" s="2">
         <v>0.92307692307692302</v>
       </c>
-      <c r="AT39" s="12" t="s">
-        <v>170</v>
+      <c r="AT39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AU39" s="15" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -4912,11 +5161,11 @@
       <c r="AR40" s="2">
         <v>0.20512820512820501</v>
       </c>
-      <c r="AT40" s="7" t="s">
-        <v>152</v>
+      <c r="AT40" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -4989,11 +5238,11 @@
       <c r="AR41" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT41" s="7" t="s">
-        <v>160</v>
+      <c r="AT41" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -5110,14 +5359,14 @@
       <c r="AR42" s="2">
         <v>0.79487179487179505</v>
       </c>
-      <c r="AT42" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="AU42" t="s">
-        <v>172</v>
+      <c r="AT42" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AU42" s="14" t="s">
+        <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -5188,11 +5437,17 @@
       <c r="AR43" s="2">
         <v>0.20512820512820501</v>
       </c>
-      <c r="AT43" s="7" t="s">
-        <v>160</v>
+      <c r="AT43" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AV43" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW43" s="38" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -5265,14 +5520,20 @@
       <c r="AR44" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT44" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU44" s="7" t="s">
+      <c r="AT44" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU44" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV44" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW44" s="37" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -5345,14 +5606,20 @@
       <c r="AR45" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT45" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU45" s="7" t="s">
+      <c r="AT45" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU45" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV45" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW45" s="37" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -5425,14 +5692,20 @@
       <c r="AR46" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT46" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU46" s="7" t="s">
+      <c r="AT46" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU46" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV46" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW46" s="37" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -5561,11 +5834,11 @@
       <c r="AR47" s="2">
         <v>0.94871794871794901</v>
       </c>
-      <c r="AT47" s="12" t="s">
-        <v>173</v>
+      <c r="AT47" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -5638,14 +5911,20 @@
       <c r="AR48" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT48" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AU48" s="7" t="s">
+      <c r="AT48" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AU48" s="14" t="s">
         <v>146</v>
       </c>
+      <c r="AV48" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW48" s="37" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -5720,11 +5999,17 @@
       <c r="AR49" s="2">
         <v>0.256410256410256</v>
       </c>
-      <c r="AT49" s="7" t="s">
-        <v>157</v>
+      <c r="AT49" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AV49" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW49" s="39" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -5797,11 +6082,20 @@
       <c r="AR50" s="2">
         <v>0.230769230769231</v>
       </c>
-      <c r="AT50" s="7" t="s">
-        <v>160</v>
+      <c r="AT50" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU50" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="AV50" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW50" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -5932,11 +6226,11 @@
       <c r="AR51" s="2">
         <v>0.97435897435897401</v>
       </c>
-      <c r="AT51" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="AU51" t="s">
-        <v>175</v>
+      <c r="AT51" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AU51" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>